<commit_message>
Roxana arreglo diccionario de datos
</commit_message>
<xml_diff>
--- a/Diccionario de datos.xlsx
+++ b/Diccionario de datos.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braya\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\MujerCuidadora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{807E4CFD-41D3-45AD-864C-E005BD6A1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BAE7D7-C56B-44D4-A521-3427FB12DD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="30960" windowHeight="12120" xr2:uid="{AB32357B-F046-458E-932F-779D260AEB8A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AB32357B-F046-458E-932F-779D260AEB8A}"/>
   </bookViews>
   <sheets>
     <sheet name="establecimientos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="101">
   <si>
     <t>Descripción</t>
   </si>
@@ -336,13 +325,16 @@
   </si>
   <si>
     <t>ID del rol del usuario.</t>
+  </si>
+  <si>
+    <t>Diccionario de Datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -351,23 +343,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -375,13 +395,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,682 +789,859 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F33F80-4400-458B-8E42-06D945035E86}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.21875" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
-    <col min="3" max="3" width="46.33203125" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B32" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B44" t="s">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C69" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C71" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B71" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B72" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C79" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B80" t="s">
-        <v>10</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="B81" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C82" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C87" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B89" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B89" t="s">
-        <v>10</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B90" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C91" s="4" t="s">
         <v>99</v>
       </c>
     </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="A68:C68"/>
+    <mergeCell ref="A77:C77"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A50:C50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>